<commit_message>
mise a jours infos
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/Resultats/confortData.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/Resultats/confortData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Bob" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,7 +13,8 @@
     <sheet name="Kevin" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Appreciation-confort" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="detendu-anxieux" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Resultats" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Aisée" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Resultats" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="30">
   <si>
     <t xml:space="preserve">confortable</t>
   </si>
@@ -105,7 +106,16 @@
     <t xml:space="preserve">V</t>
   </si>
   <si>
+    <t xml:space="preserve">Effect Size</t>
+  </si>
+  <si>
     <t xml:space="preserve">Confort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detendu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxieux</t>
   </si>
 </sst>
 </file>
@@ -115,7 +125,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -136,6 +146,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -213,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -222,7 +239,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -230,11 +251,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,7 +263,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -266,7 +287,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -1596,7 +1617,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -2865,7 +2886,7 @@
   <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -4133,7 +4154,7 @@
   </sheetPr>
   <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A124" activeCellId="0" sqref="A124"/>
     </sheetView>
   </sheetViews>
@@ -5512,16 +5533,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5051020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5543,6 +5565,15 @@
       <c r="F1" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -5563,6 +5594,17 @@
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">C2</f>
+        <v>4</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">E2</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -5583,6 +5625,17 @@
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">C3</f>
+        <v>5</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">E3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -5603,6 +5656,17 @@
       <c r="F4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <f aca="false">C4</f>
+        <v>3</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <f aca="false">E4</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -5623,6 +5687,17 @@
       <c r="F5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">C5</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">E5</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -5643,6 +5718,17 @@
       <c r="F6" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">C6</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">E6</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -5663,6 +5749,17 @@
       <c r="F7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <f aca="false">C7</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">E7</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -5683,6 +5780,17 @@
       <c r="F8" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">C8</f>
+        <v>2</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">E8</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -5703,6 +5811,17 @@
       <c r="F9" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">C9</f>
+        <v>2</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">E9</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -5723,6 +5842,17 @@
       <c r="F10" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <f aca="false">C10</f>
+        <v>2</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <f aca="false">E10</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -5743,6 +5873,17 @@
       <c r="F11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <f aca="false">C11</f>
+        <v>5</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">E11</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -5763,6 +5904,17 @@
       <c r="F12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <f aca="false">C12</f>
+        <v>5</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">E12</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -5783,6 +5935,17 @@
       <c r="F13" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <f aca="false">C13</f>
+        <v>3</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">E13</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -5803,6 +5966,17 @@
       <c r="F14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">C14</f>
+        <v>2</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">E14</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -5823,6 +5997,17 @@
       <c r="F15" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">C15</f>
+        <v>4</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">E15</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -5843,6 +6028,17 @@
       <c r="F16" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">C16</f>
+        <v>3</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <f aca="false">E16</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -5863,6 +6059,17 @@
       <c r="F17" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">C17</f>
+        <v>4</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">E17</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -5883,6 +6090,17 @@
       <c r="F18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G18" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">C18</f>
+        <v>4</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">E18</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -5903,6 +6121,17 @@
       <c r="F19" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">C19</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">E19</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -5923,6 +6152,17 @@
       <c r="F20" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">C20</f>
+        <v>2</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">E20</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -5943,6 +6183,17 @@
       <c r="F21" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">C21</f>
+        <v>4</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">E21</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -5963,6 +6214,17 @@
       <c r="F22" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">C22</f>
+        <v>5</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <f aca="false">E22</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -5983,6 +6245,17 @@
       <c r="F23" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">C23</f>
+        <v>3</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <f aca="false">E23</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
@@ -6003,6 +6276,17 @@
       <c r="F24" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">C24</f>
+        <v>5</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <f aca="false">E24</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -6023,6 +6307,17 @@
       <c r="F25" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">C25</f>
+        <v>2</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <f aca="false">E25</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -6043,6 +6338,17 @@
       <c r="F26" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">C26</f>
+        <v>3</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <f aca="false">E26</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -6063,6 +6369,17 @@
       <c r="F27" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">C27</f>
+        <v>3</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">E27</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -6083,6 +6400,17 @@
       <c r="F28" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <f aca="false">C28</f>
+        <v>3</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <f aca="false">E28</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
@@ -6103,6 +6431,17 @@
       <c r="F29" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G29" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">C29</f>
+        <v>4</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <f aca="false">E29</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -6123,6 +6462,17 @@
       <c r="F30" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G30" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">C30</f>
+        <v>4</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <f aca="false">E30</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -6143,6 +6493,17 @@
       <c r="F31" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <f aca="false">C31</f>
+        <v>5</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <f aca="false">E31</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -6163,6 +6524,17 @@
       <c r="F32" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <f aca="false">C32</f>
+        <v>5</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <f aca="false">E32</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -6183,6 +6555,17 @@
       <c r="F33" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G33" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">C33</f>
+        <v>4</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">E33</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -6203,6 +6586,17 @@
       <c r="F34" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G34" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <f aca="false">C34</f>
+        <v>4</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <f aca="false">E34</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -6223,6 +6617,17 @@
       <c r="F35" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <f aca="false">C35</f>
+        <v>4</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <f aca="false">E35</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -6243,6 +6648,17 @@
       <c r="F36" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <f aca="false">C36</f>
+        <v>4</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <f aca="false">E36</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -6263,6 +6679,17 @@
       <c r="F37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <f aca="false">C37</f>
+        <v>5</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <f aca="false">E37</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -6283,6 +6710,17 @@
       <c r="F38" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <f aca="false">C38</f>
+        <v>5</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <f aca="false">E38</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -6303,6 +6741,17 @@
       <c r="F39" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G39" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <f aca="false">C39</f>
+        <v>4</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <f aca="false">E39</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -6323,6 +6772,17 @@
       <c r="F40" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <f aca="false">C40</f>
+        <v>2</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <f aca="false">E40</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -6343,6 +6803,17 @@
       <c r="F41" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G41" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <f aca="false">C41</f>
+        <v>2</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <f aca="false">E41</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -6363,6 +6834,17 @@
       <c r="F42" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G42" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <f aca="false">C42</f>
+        <v>5</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <f aca="false">E42</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
@@ -6383,6 +6865,17 @@
       <c r="F43" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <f aca="false">C43</f>
+        <v>1</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <f aca="false">E43</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
@@ -6403,6 +6896,17 @@
       <c r="F44" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G44" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <f aca="false">C44</f>
+        <v>2</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <f aca="false">E44</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
@@ -6423,6 +6927,17 @@
       <c r="F45" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G45" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <f aca="false">C45</f>
+        <v>2</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <f aca="false">E45</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
@@ -6443,6 +6958,17 @@
       <c r="F46" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="G46" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <f aca="false">C46</f>
+        <v>1</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <f aca="false">E46</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
@@ -6463,6 +6989,17 @@
       <c r="F47" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <f aca="false">C47</f>
+        <v>5</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <f aca="false">E47</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
@@ -6483,6 +7020,17 @@
       <c r="F48" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G48" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <f aca="false">C48</f>
+        <v>5</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <f aca="false">E48</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
@@ -6503,6 +7051,17 @@
       <c r="F49" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G49" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <f aca="false">C49</f>
+        <v>5</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <f aca="false">E49</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
@@ -6523,6 +7082,17 @@
       <c r="F50" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <f aca="false">C50</f>
+        <v>4</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <f aca="false">E50</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
@@ -6543,6 +7113,17 @@
       <c r="F51" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <f aca="false">C51</f>
+        <v>4</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <f aca="false">E51</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
@@ -6563,6 +7144,17 @@
       <c r="F52" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G52" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <f aca="false">C52</f>
+        <v>5</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <f aca="false">E52</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
@@ -6583,6 +7175,17 @@
       <c r="F53" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G53" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <f aca="false">C53</f>
+        <v>4</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <f aca="false">E53</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
@@ -6603,6 +7206,17 @@
       <c r="F54" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <f aca="false">C54</f>
+        <v>2</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <f aca="false">E54</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
@@ -6623,6 +7237,17 @@
       <c r="F55" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="G55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <f aca="false">C55</f>
+        <v>4</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <f aca="false">E55</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
@@ -6643,6 +7268,17 @@
       <c r="F56" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G56" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <f aca="false">C56</f>
+        <v>4</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <f aca="false">E56</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
@@ -6663,6 +7299,17 @@
       <c r="F57" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G57" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <f aca="false">C57</f>
+        <v>3</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <f aca="false">E57</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
@@ -6683,6 +7330,17 @@
       <c r="F58" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <f aca="false">C58</f>
+        <v>5</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <f aca="false">E58</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
@@ -6703,6 +7361,17 @@
       <c r="F59" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G59" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <f aca="false">C59</f>
+        <v>2</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <f aca="false">E59</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
@@ -6723,6 +7392,17 @@
       <c r="F60" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="G60" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <f aca="false">C60</f>
+        <v>2</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <f aca="false">E60</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
@@ -6743,6 +7423,17 @@
       <c r="F61" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <f aca="false">C61</f>
+        <v>4</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <f aca="false">E61</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
@@ -6762,6 +7453,871 @@
       </c>
       <c r="F62" s="0" t="n">
         <v>2</v>
+      </c>
+      <c r="G62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <f aca="false">C62</f>
+        <v>2</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <f aca="false">E62</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G63" s="0" t="n">
+        <f aca="false">6-B2</f>
+        <v>5</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <f aca="false">6-D2</f>
+        <v>4</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <f aca="false">6-F2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G64" s="0" t="n">
+        <f aca="false">6-B3</f>
+        <v>5</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <f aca="false">6-D3</f>
+        <v>5</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <f aca="false">6-F3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G65" s="0" t="n">
+        <f aca="false">6-B4</f>
+        <v>3</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <f aca="false">6-D4</f>
+        <v>4</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <f aca="false">6-F4</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G66" s="0" t="n">
+        <f aca="false">6-B5</f>
+        <v>5</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <f aca="false">6-D5</f>
+        <v>5</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <f aca="false">6-F5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G67" s="0" t="n">
+        <f aca="false">6-B6</f>
+        <v>3</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <f aca="false">6-D6</f>
+        <v>5</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <f aca="false">6-F6</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G68" s="0" t="n">
+        <f aca="false">6-B7</f>
+        <v>4</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <f aca="false">6-D7</f>
+        <v>3</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <f aca="false">6-F7</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G69" s="0" t="n">
+        <f aca="false">6-B8</f>
+        <v>3</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <f aca="false">6-D8</f>
+        <v>2</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <f aca="false">6-F8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G70" s="0" t="n">
+        <f aca="false">6-B9</f>
+        <v>5</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <f aca="false">6-D9</f>
+        <v>5</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <f aca="false">6-F9</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G71" s="0" t="n">
+        <f aca="false">6-B10</f>
+        <v>4</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <f aca="false">6-D10</f>
+        <v>3</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <f aca="false">6-F10</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G72" s="0" t="n">
+        <f aca="false">6-B11</f>
+        <v>5</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <f aca="false">6-D11</f>
+        <v>5</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <f aca="false">6-F11</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G73" s="0" t="n">
+        <f aca="false">6-B12</f>
+        <v>5</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <f aca="false">6-D12</f>
+        <v>5</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <f aca="false">6-F12</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="0" t="n">
+        <f aca="false">6-B13</f>
+        <v>4</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <f aca="false">6-D13</f>
+        <v>3</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <f aca="false">6-F13</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G75" s="0" t="n">
+        <f aca="false">6-B14</f>
+        <v>5</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <f aca="false">6-D14</f>
+        <v>2</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <f aca="false">6-F14</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G76" s="0" t="n">
+        <f aca="false">6-B15</f>
+        <v>5</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <f aca="false">6-D15</f>
+        <v>4</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <f aca="false">6-F15</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G77" s="0" t="n">
+        <f aca="false">6-B16</f>
+        <v>4</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <f aca="false">6-D16</f>
+        <v>4</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <f aca="false">6-F16</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G78" s="0" t="n">
+        <f aca="false">6-B17</f>
+        <v>3</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <f aca="false">6-D17</f>
+        <v>4</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <f aca="false">6-F17</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G79" s="0" t="n">
+        <f aca="false">6-B18</f>
+        <v>5</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <f aca="false">6-D18</f>
+        <v>4</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <f aca="false">6-F18</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G80" s="0" t="n">
+        <f aca="false">6-B19</f>
+        <v>5</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <f aca="false">6-D19</f>
+        <v>2</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <f aca="false">6-F19</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G81" s="0" t="n">
+        <f aca="false">6-B20</f>
+        <v>3</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <f aca="false">6-D20</f>
+        <v>2</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <f aca="false">6-F20</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G82" s="0" t="n">
+        <f aca="false">6-B21</f>
+        <v>4</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <f aca="false">6-D21</f>
+        <v>4</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <f aca="false">6-F21</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G83" s="0" t="n">
+        <f aca="false">6-B22</f>
+        <v>3</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <f aca="false">6-D22</f>
+        <v>3</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <f aca="false">6-F22</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G84" s="0" t="n">
+        <f aca="false">6-B23</f>
+        <v>3</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <f aca="false">6-D23</f>
+        <v>3</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <f aca="false">6-F23</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G85" s="0" t="n">
+        <f aca="false">6-B24</f>
+        <v>5</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <f aca="false">6-D24</f>
+        <v>5</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <f aca="false">6-F24</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G86" s="0" t="n">
+        <f aca="false">6-B25</f>
+        <v>4</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <f aca="false">6-D25</f>
+        <v>2</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <f aca="false">6-F25</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G87" s="0" t="n">
+        <f aca="false">6-B26</f>
+        <v>5</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <f aca="false">6-D26</f>
+        <v>5</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <f aca="false">6-F26</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G88" s="0" t="n">
+        <f aca="false">6-B27</f>
+        <v>5</v>
+      </c>
+      <c r="H88" s="0" t="n">
+        <f aca="false">6-D27</f>
+        <v>5</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <f aca="false">6-F27</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G89" s="0" t="n">
+        <f aca="false">6-B28</f>
+        <v>4</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <f aca="false">6-D28</f>
+        <v>4</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <f aca="false">6-F28</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G90" s="0" t="n">
+        <f aca="false">6-B29</f>
+        <v>4</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <f aca="false">6-D29</f>
+        <v>4</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <f aca="false">6-F29</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G91" s="0" t="n">
+        <f aca="false">6-B30</f>
+        <v>4</v>
+      </c>
+      <c r="H91" s="0" t="n">
+        <f aca="false">6-D30</f>
+        <v>4</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <f aca="false">6-F30</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G92" s="0" t="n">
+        <f aca="false">6-B31</f>
+        <v>4</v>
+      </c>
+      <c r="H92" s="0" t="n">
+        <f aca="false">6-D31</f>
+        <v>4</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <f aca="false">6-F31</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G93" s="0" t="n">
+        <f aca="false">6-B32</f>
+        <v>5</v>
+      </c>
+      <c r="H93" s="0" t="n">
+        <f aca="false">6-D32</f>
+        <v>5</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <f aca="false">6-F32</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G94" s="0" t="n">
+        <f aca="false">6-B33</f>
+        <v>5</v>
+      </c>
+      <c r="H94" s="0" t="n">
+        <f aca="false">6-D33</f>
+        <v>5</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <f aca="false">6-F33</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G95" s="0" t="n">
+        <f aca="false">6-B34</f>
+        <v>4</v>
+      </c>
+      <c r="H95" s="0" t="n">
+        <f aca="false">6-D34</f>
+        <v>4</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <f aca="false">6-F34</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G96" s="0" t="n">
+        <f aca="false">6-B35</f>
+        <v>4</v>
+      </c>
+      <c r="H96" s="0" t="n">
+        <f aca="false">6-D35</f>
+        <v>4</v>
+      </c>
+      <c r="I96" s="0" t="n">
+        <f aca="false">6-F35</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G97" s="0" t="n">
+        <f aca="false">6-B36</f>
+        <v>5</v>
+      </c>
+      <c r="H97" s="0" t="n">
+        <f aca="false">6-D36</f>
+        <v>4</v>
+      </c>
+      <c r="I97" s="0" t="n">
+        <f aca="false">6-F36</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G98" s="0" t="n">
+        <f aca="false">6-B37</f>
+        <v>5</v>
+      </c>
+      <c r="H98" s="0" t="n">
+        <f aca="false">6-D37</f>
+        <v>5</v>
+      </c>
+      <c r="I98" s="0" t="n">
+        <f aca="false">6-F37</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G99" s="0" t="n">
+        <f aca="false">6-B38</f>
+        <v>4</v>
+      </c>
+      <c r="H99" s="0" t="n">
+        <f aca="false">6-D38</f>
+        <v>5</v>
+      </c>
+      <c r="I99" s="0" t="n">
+        <f aca="false">6-F38</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G100" s="0" t="n">
+        <f aca="false">6-B39</f>
+        <v>2</v>
+      </c>
+      <c r="H100" s="0" t="n">
+        <f aca="false">6-D39</f>
+        <v>4</v>
+      </c>
+      <c r="I100" s="0" t="n">
+        <f aca="false">6-F39</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G101" s="0" t="n">
+        <f aca="false">6-B40</f>
+        <v>2</v>
+      </c>
+      <c r="H101" s="0" t="n">
+        <f aca="false">6-D40</f>
+        <v>4</v>
+      </c>
+      <c r="I101" s="0" t="n">
+        <f aca="false">6-F40</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G102" s="0" t="n">
+        <f aca="false">6-B41</f>
+        <v>5</v>
+      </c>
+      <c r="H102" s="0" t="n">
+        <f aca="false">6-D41</f>
+        <v>2</v>
+      </c>
+      <c r="I102" s="0" t="n">
+        <f aca="false">6-F41</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G103" s="0" t="n">
+        <f aca="false">6-B42</f>
+        <v>5</v>
+      </c>
+      <c r="H103" s="0" t="n">
+        <f aca="false">6-D42</f>
+        <v>4</v>
+      </c>
+      <c r="I103" s="0" t="n">
+        <f aca="false">6-F42</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G104" s="0" t="n">
+        <f aca="false">6-B43</f>
+        <v>4</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <f aca="false">6-D43</f>
+        <v>4</v>
+      </c>
+      <c r="I104" s="0" t="n">
+        <f aca="false">6-F43</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G105" s="0" t="n">
+        <f aca="false">6-B44</f>
+        <v>5</v>
+      </c>
+      <c r="H105" s="0" t="n">
+        <f aca="false">6-D44</f>
+        <v>3</v>
+      </c>
+      <c r="I105" s="0" t="n">
+        <f aca="false">6-F44</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G106" s="0" t="n">
+        <f aca="false">6-B45</f>
+        <v>5</v>
+      </c>
+      <c r="H106" s="0" t="n">
+        <f aca="false">6-D45</f>
+        <v>4</v>
+      </c>
+      <c r="I106" s="0" t="n">
+        <f aca="false">6-F45</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G107" s="0" t="n">
+        <f aca="false">6-B46</f>
+        <v>3</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <f aca="false">6-D46</f>
+        <v>2</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <f aca="false">6-F46</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G108" s="0" t="n">
+        <f aca="false">6-B47</f>
+        <v>5</v>
+      </c>
+      <c r="H108" s="0" t="n">
+        <f aca="false">6-D47</f>
+        <v>5</v>
+      </c>
+      <c r="I108" s="0" t="n">
+        <f aca="false">6-F47</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G109" s="0" t="n">
+        <f aca="false">6-B48</f>
+        <v>5</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <f aca="false">6-D48</f>
+        <v>5</v>
+      </c>
+      <c r="I109" s="0" t="n">
+        <f aca="false">6-F48</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G110" s="0" t="n">
+        <f aca="false">6-B49</f>
+        <v>4</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <f aca="false">6-D49</f>
+        <v>5</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <f aca="false">6-F49</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G111" s="0" t="n">
+        <f aca="false">6-B50</f>
+        <v>5</v>
+      </c>
+      <c r="H111" s="0" t="n">
+        <f aca="false">6-D50</f>
+        <v>5</v>
+      </c>
+      <c r="I111" s="0" t="n">
+        <f aca="false">6-F50</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G112" s="0" t="n">
+        <f aca="false">6-B51</f>
+        <v>4</v>
+      </c>
+      <c r="H112" s="0" t="n">
+        <f aca="false">6-D51</f>
+        <v>4</v>
+      </c>
+      <c r="I112" s="0" t="n">
+        <f aca="false">6-F51</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G113" s="0" t="n">
+        <f aca="false">6-B52</f>
+        <v>5</v>
+      </c>
+      <c r="H113" s="0" t="n">
+        <f aca="false">6-D52</f>
+        <v>5</v>
+      </c>
+      <c r="I113" s="0" t="n">
+        <f aca="false">6-F52</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G114" s="0" t="n">
+        <f aca="false">6-B53</f>
+        <v>4</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <f aca="false">6-D53</f>
+        <v>3</v>
+      </c>
+      <c r="I114" s="0" t="n">
+        <f aca="false">6-F53</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G115" s="0" t="n">
+        <f aca="false">6-B54</f>
+        <v>4</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <f aca="false">6-D54</f>
+        <v>5</v>
+      </c>
+      <c r="I115" s="0" t="n">
+        <f aca="false">6-F54</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G116" s="0" t="n">
+        <f aca="false">6-B55</f>
+        <v>2</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <f aca="false">6-D55</f>
+        <v>2</v>
+      </c>
+      <c r="I116" s="0" t="n">
+        <f aca="false">6-F55</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G117" s="0" t="n">
+        <f aca="false">6-B56</f>
+        <v>5</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <f aca="false">6-D56</f>
+        <v>3</v>
+      </c>
+      <c r="I117" s="0" t="n">
+        <f aca="false">6-F56</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G118" s="0" t="n">
+        <f aca="false">6-B57</f>
+        <v>3</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <f aca="false">6-D57</f>
+        <v>3</v>
+      </c>
+      <c r="I118" s="0" t="n">
+        <f aca="false">6-F57</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G119" s="0" t="n">
+        <f aca="false">6-B58</f>
+        <v>5</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <f aca="false">6-D58</f>
+        <v>5</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <f aca="false">6-F58</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G120" s="0" t="n">
+        <f aca="false">6-B59</f>
+        <v>5</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <f aca="false">6-D59</f>
+        <v>2</v>
+      </c>
+      <c r="I120" s="0" t="n">
+        <f aca="false">6-F59</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G121" s="0" t="n">
+        <f aca="false">6-B60</f>
+        <v>4</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <f aca="false">6-D60</f>
+        <v>4</v>
+      </c>
+      <c r="I121" s="0" t="n">
+        <f aca="false">6-F60</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G122" s="0" t="n">
+        <f aca="false">6-B61</f>
+        <v>5</v>
+      </c>
+      <c r="H122" s="0" t="n">
+        <f aca="false">6-D61</f>
+        <v>4</v>
+      </c>
+      <c r="I122" s="0" t="n">
+        <f aca="false">6-F61</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G123" s="0" t="n">
+        <f aca="false">6-B62</f>
+        <v>3</v>
+      </c>
+      <c r="H123" s="0" t="n">
+        <f aca="false">6-D62</f>
+        <v>3</v>
+      </c>
+      <c r="I123" s="0" t="n">
+        <f aca="false">6-F62</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6780,10 +8336,720 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:C62"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C48" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C49" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C51" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C52" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C53" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C54" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C55" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C56" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C57" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C58" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C61" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -6878,140 +9144,270 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="I12" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3" t="n">
+      <c r="B13" s="4" t="n">
         <v>3.827869</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>3.459016</v>
       </c>
-      <c r="D13" s="3" t="n">
+      <c r="D13" s="4" t="n">
         <v>3.852459</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="3" t="n">
+      <c r="G13" s="4" t="n">
         <v>2026</v>
       </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>0.0005365</v>
       </c>
+      <c r="I13" s="4" t="n">
+        <v>0.2031699</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3" t="n">
+      <c r="B14" s="4" t="n">
         <v>1.01796</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="4" t="n">
         <v>1.092026</v>
       </c>
-      <c r="D14" s="3" t="n">
+      <c r="D14" s="4" t="n">
         <v>1.025881</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="3" t="n">
+      <c r="G14" s="4" t="n">
         <v>1154.5</v>
       </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>0.6298</v>
       </c>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="3" t="n">
+      <c r="G15" s="4" t="n">
         <v>1901</v>
       </c>
-      <c r="H15" s="3" t="n">
+      <c r="H15" s="4" t="n">
         <v>0.0003304</v>
       </c>
+      <c r="I15" s="4" t="n">
+        <v>0.2108808</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="6" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="7" t="n">
+        <v>3.672131</v>
+      </c>
+      <c r="D18" s="7" t="n">
+        <v>3.92623</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="7" t="n">
+        <v>1449</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <v>0.002568</v>
+      </c>
+      <c r="I18" s="7" t="n">
+        <v>-0.1751026</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="n">
+        <v>0.9706435</v>
+      </c>
+      <c r="C19" s="7" t="n">
+        <v>1.145906</v>
+      </c>
+      <c r="D19" s="7" t="n">
+        <v>1.06924</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>749</v>
+      </c>
+      <c r="H19" s="7" t="n">
+        <v>0.2006</v>
+      </c>
+      <c r="I19" s="7" t="n">
+        <v>-0.05160643</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="7" t="n">
+        <v>942.5</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <v>1.003483</v>
+      </c>
+      <c r="I20" s="7" t="n">
+        <v>-0.1677209</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="F18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6" t="s">
+      <c r="B22" s="7" t="n">
+        <v>3.786885</v>
+      </c>
+      <c r="C22" s="7" t="n">
+        <v>3.47541</v>
+      </c>
+      <c r="D22" s="7" t="n">
+        <v>3.786885</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="F19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F20" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="B23" s="7" t="n">
+        <v>1.001911</v>
+      </c>
+      <c r="C23" s="7" t="n">
+        <v>1.219379</v>
+      </c>
+      <c r="D23" s="7" t="n">
+        <v>1.09719</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>1.786885</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>2.131148</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>1.934426</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="7" t="n">
+        <v>0.896563</v>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>1.040439</v>
+      </c>
+      <c r="D28" s="7" t="n">
+        <v>1.030677</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
MIES A JOURS DES DONNES DE CONFORT
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/Resultats/confortData.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/Resultats/confortData.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Bob" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Arthur" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Kevin" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Appreciation-confort" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Appreciation" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="detendu-anxieux" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Aisée" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Resultats" sheetId="7" state="visible" r:id="rId8"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="32">
   <si>
     <t xml:space="preserve">confortable</t>
   </si>
@@ -120,15 +120,19 @@
   <si>
     <t xml:space="preserve">Anxieux</t>
   </si>
+  <si>
+    <t xml:space="preserve">Aisée</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -171,8 +175,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +198,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00CCFF"/>
         <bgColor rgb="FF33CCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -233,7 +248,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -270,6 +285,26 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -279,6 +314,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -295,9 +390,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1625,9 +1721,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.219387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,9 +2991,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,14 +4255,14 @@
   </sheetPr>
   <dimension ref="A1:C123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A124" activeCellId="0" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5538,15 +5636,15 @@
   </sheetPr>
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C61" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8341,14 +8439,14 @@
   </sheetPr>
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="30.5102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9049,18 +9147,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I33" activeCellId="0" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.5051020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="10.9336734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9198,9 +9296,11 @@
         <v>0.0005365</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>0.2031699</v>
-      </c>
-      <c r="J13" s="4"/>
+        <v>-0.2031699</v>
+      </c>
+      <c r="J13" s="4" t="n">
+        <v>-3.173615</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
@@ -9224,8 +9324,12 @@
       <c r="H14" s="4" t="n">
         <v>0.6298</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="4" t="n">
+        <v>-0.02028643</v>
+      </c>
+      <c r="J14" s="4" t="n">
+        <v>-0.3168842</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F15" s="4" t="s">
@@ -9238,9 +9342,11 @@
         <v>0.0003304</v>
       </c>
       <c r="I15" s="4" t="n">
-        <v>0.2108808</v>
-      </c>
-      <c r="J15" s="4"/>
+        <v>-0.2108808</v>
+      </c>
+      <c r="J15" s="4" t="n">
+        <v>-3.294064</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
@@ -9296,7 +9402,9 @@
       <c r="I18" s="7" t="n">
         <v>-0.1751026</v>
       </c>
-      <c r="J18" s="7"/>
+      <c r="J18" s="7" t="n">
+        <v>-2.735189</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
@@ -9323,7 +9431,9 @@
       <c r="I19" s="7" t="n">
         <v>-0.05160643</v>
       </c>
-      <c r="J19" s="7"/>
+      <c r="J19" s="7" t="n">
+        <v>-0.8061182</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="7" t="s">
@@ -9338,7 +9448,9 @@
       <c r="I20" s="7" t="n">
         <v>-0.1677209</v>
       </c>
-      <c r="J20" s="7"/>
+      <c r="J20" s="7" t="n">
+        <v>-2.619884</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
@@ -9422,6 +9534,104 @@
       </c>
       <c r="D28" s="7" t="n">
         <v>1.030677</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>3.163934</v>
+      </c>
+      <c r="D32" s="12" t="n">
+        <v>3.901639</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G32" s="10"/>
+      <c r="H32" s="13" t="n">
+        <v>4.281E-005</v>
+      </c>
+      <c r="I32" s="10" t="n">
+        <v>-0.3498287</v>
+      </c>
+      <c r="J32" s="10" t="n">
+        <v>-3.863985</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="n">
+        <v>1.098185</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>0.9950698</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10" t="n">
+        <v>0.1718</v>
+      </c>
+      <c r="I33" s="10" t="n">
+        <v>-0.08210674</v>
+      </c>
+      <c r="J33" s="10" t="n">
+        <v>-0.9068986</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F34" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10" t="n">
+        <v>0.0001158</v>
+      </c>
+      <c r="I34" s="10" t="n">
+        <v>-0.3272274</v>
+      </c>
+      <c r="J34" s="10" t="n">
+        <v>-3.614344</v>
       </c>
     </row>
   </sheetData>

</xml_diff>